<commit_message>
Add new Waves5 indicator, new sample data, new docs, include LKN and NLWKN station.
The software for the DWR stations is gradually being changed from Waves21 to Waves5 (Datawell). This changes the definition of the timestamp for the *.his and *GPS.txt files from "reception time at the measuring computer" to "end time of the measuring period".

As a new sample data station FINO1 (16th November 2024) was chosen because there are measurements for all three sensors.

There are new versions of the documentations.

Include new LKN and NLWKN DWR stations.

For stations FN1 and BO1, periods with poor RADAC measurements were set to FQF=4.
</commit_message>
<xml_diff>
--- a/02_work/Metadatenbank.xlsx
+++ b/02_work/Metadatenbank.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MATLAB\DQC_Server\work\Jobs\DQC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\work\Jobs\DQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76E4F69-70C0-4710-A743-20657AE15CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19905" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="29295" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DWR" sheetId="1" r:id="rId1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="188">
   <si>
     <t>tlower</t>
   </si>
@@ -579,11 +580,29 @@
   <si>
     <t>Stohl</t>
   </si>
+  <si>
+    <t>N13N</t>
+  </si>
+  <si>
+    <t>Vorhabengebiet 13 Nord</t>
+  </si>
+  <si>
+    <t>N13S</t>
+  </si>
+  <si>
+    <t>Vorhabengebiet 13 Sued</t>
+  </si>
+  <si>
+    <t>N68</t>
+  </si>
+  <si>
+    <t>Vorhabengebiet 68</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -939,16 +958,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DU29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:DU33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="5"/>
+    <col min="1" max="1" width="11.625" style="5" customWidth="1"/>
     <col min="2" max="2" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8140,13 +8159,13 @@
         <v>165</v>
       </c>
       <c r="C21" s="4">
-        <v>54.005890000000001</v>
+        <v>53.749499999999998</v>
       </c>
       <c r="D21" s="4">
-        <v>6.6128</v>
+        <v>7.1186999999999996</v>
       </c>
       <c r="E21" s="2">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F21" s="1">
         <v>39814</v>
@@ -9588,7 +9607,7 @@
         <v>44954</v>
       </c>
       <c r="G25" s="1">
-        <v>2958465</v>
+        <v>45123</v>
       </c>
       <c r="H25" s="3">
         <v>0.01</v>
@@ -9947,7 +9966,7 @@
         <v>44954</v>
       </c>
       <c r="G26" s="1">
-        <v>2958465</v>
+        <v>45123</v>
       </c>
       <c r="H26" s="3">
         <v>0.01</v>
@@ -11336,8 +11355,1061 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="30" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" s="4">
+        <v>55.099583000000003</v>
+      </c>
+      <c r="D30" s="4">
+        <v>6.3000220000000002</v>
+      </c>
+      <c r="E30" s="12">
+        <v>42</v>
+      </c>
+      <c r="F30" s="1">
+        <v>45456</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2958465</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="J30" s="3">
+        <v>-20</v>
+      </c>
+      <c r="K30" s="3">
+        <v>20</v>
+      </c>
+      <c r="L30" s="3">
+        <v>-15</v>
+      </c>
+      <c r="M30" s="3">
+        <v>15</v>
+      </c>
+      <c r="N30" s="3">
+        <v>0</v>
+      </c>
+      <c r="O30" s="3">
+        <v>25</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>40</v>
+      </c>
+      <c r="R30" s="3">
+        <v>0</v>
+      </c>
+      <c r="S30" s="3">
+        <v>40</v>
+      </c>
+      <c r="T30" s="3">
+        <v>0</v>
+      </c>
+      <c r="U30" s="3">
+        <v>25</v>
+      </c>
+      <c r="V30" s="3">
+        <v>0</v>
+      </c>
+      <c r="W30" s="3">
+        <v>25</v>
+      </c>
+      <c r="X30" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>30</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="3">
+        <v>25</v>
+      </c>
+      <c r="AB30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE30" s="3">
+        <v>30</v>
+      </c>
+      <c r="AF30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG30" s="3">
+        <v>25</v>
+      </c>
+      <c r="AH30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI30" s="3">
+        <v>30</v>
+      </c>
+      <c r="AJ30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK30" s="3">
+        <v>30</v>
+      </c>
+      <c r="AL30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM30" s="3">
+        <v>30</v>
+      </c>
+      <c r="AN30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AO30" s="3">
+        <v>30</v>
+      </c>
+      <c r="AP30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AQ30" s="3">
+        <v>30</v>
+      </c>
+      <c r="AR30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS30" s="3">
+        <v>360</v>
+      </c>
+      <c r="AT30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU30" s="3">
+        <v>360</v>
+      </c>
+      <c r="AV30" s="3">
+        <v>-2</v>
+      </c>
+      <c r="AW30" s="3">
+        <v>32</v>
+      </c>
+      <c r="AX30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY30" s="3">
+        <v>1</v>
+      </c>
+      <c r="AZ30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BA30" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC30" s="3">
+        <v>1</v>
+      </c>
+      <c r="BD30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE30" s="3">
+        <v>7</v>
+      </c>
+      <c r="BF30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG30" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="BH30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BI30" s="3">
+        <v>500</v>
+      </c>
+      <c r="BJ30" s="3">
+        <v>3</v>
+      </c>
+      <c r="BK30" s="3">
+        <v>3</v>
+      </c>
+      <c r="BL30" s="3">
+        <v>3</v>
+      </c>
+      <c r="BM30" s="3">
+        <v>3</v>
+      </c>
+      <c r="BN30" s="3">
+        <v>3</v>
+      </c>
+      <c r="BO30" s="3">
+        <v>10</v>
+      </c>
+      <c r="BP30" s="3">
+        <v>4</v>
+      </c>
+      <c r="BQ30" s="3">
+        <v>4</v>
+      </c>
+      <c r="BR30" s="3">
+        <v>4</v>
+      </c>
+      <c r="BS30" s="3">
+        <v>4</v>
+      </c>
+      <c r="BT30" s="3">
+        <v>4</v>
+      </c>
+      <c r="BU30" s="3">
+        <v>4</v>
+      </c>
+      <c r="BV30" s="3">
+        <v>4</v>
+      </c>
+      <c r="BW30" s="3">
+        <v>10</v>
+      </c>
+      <c r="BX30" s="3">
+        <v>4</v>
+      </c>
+      <c r="BY30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="BZ30" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CA30" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="CB30" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="CC30" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="CD30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CE30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CF30" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CG30" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CH30" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CI30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CJ30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CK30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CL30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CM30" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CN30" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="CO30" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="CP30" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CQ30" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CR30" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CS30" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="CT30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CU30" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="CV30" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="CW30" s="3">
+        <v>3</v>
+      </c>
+      <c r="CX30" s="3">
+        <v>3</v>
+      </c>
+      <c r="CY30" s="3">
+        <v>3</v>
+      </c>
+      <c r="CZ30" s="3">
+        <v>3</v>
+      </c>
+      <c r="DA30" s="3">
+        <v>3</v>
+      </c>
+      <c r="DB30" s="3">
+        <v>10</v>
+      </c>
+      <c r="DC30" s="3">
+        <v>4</v>
+      </c>
+      <c r="DD30" s="3">
+        <v>4</v>
+      </c>
+      <c r="DE30" s="3">
+        <v>4</v>
+      </c>
+      <c r="DF30" s="3">
+        <v>4</v>
+      </c>
+      <c r="DG30" s="3">
+        <v>4</v>
+      </c>
+      <c r="DH30" s="3">
+        <v>4</v>
+      </c>
+      <c r="DI30" s="3">
+        <v>4</v>
+      </c>
+      <c r="DJ30" s="3">
+        <v>10</v>
+      </c>
+      <c r="DK30" s="3">
+        <v>4</v>
+      </c>
+      <c r="DL30" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="31" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C31" s="4">
+        <v>54.979595000000003</v>
+      </c>
+      <c r="D31" s="4">
+        <v>6.2999980000000004</v>
+      </c>
+      <c r="E31" s="12">
+        <v>39</v>
+      </c>
+      <c r="F31" s="1">
+        <v>45456</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2958465</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="J31" s="3">
+        <v>-20</v>
+      </c>
+      <c r="K31" s="3">
+        <v>20</v>
+      </c>
+      <c r="L31" s="3">
+        <v>-15</v>
+      </c>
+      <c r="M31" s="3">
+        <v>15</v>
+      </c>
+      <c r="N31" s="3">
+        <v>0</v>
+      </c>
+      <c r="O31" s="3">
+        <v>25</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>40</v>
+      </c>
+      <c r="R31" s="3">
+        <v>0</v>
+      </c>
+      <c r="S31" s="3">
+        <v>40</v>
+      </c>
+      <c r="T31" s="3">
+        <v>0</v>
+      </c>
+      <c r="U31" s="3">
+        <v>25</v>
+      </c>
+      <c r="V31" s="3">
+        <v>0</v>
+      </c>
+      <c r="W31" s="3">
+        <v>25</v>
+      </c>
+      <c r="X31" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>30</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>25</v>
+      </c>
+      <c r="AB31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE31" s="3">
+        <v>30</v>
+      </c>
+      <c r="AF31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="3">
+        <v>25</v>
+      </c>
+      <c r="AH31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI31" s="3">
+        <v>30</v>
+      </c>
+      <c r="AJ31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK31" s="3">
+        <v>30</v>
+      </c>
+      <c r="AL31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM31" s="3">
+        <v>30</v>
+      </c>
+      <c r="AN31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AO31" s="3">
+        <v>30</v>
+      </c>
+      <c r="AP31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AQ31" s="3">
+        <v>30</v>
+      </c>
+      <c r="AR31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS31" s="3">
+        <v>360</v>
+      </c>
+      <c r="AT31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU31" s="3">
+        <v>360</v>
+      </c>
+      <c r="AV31" s="3">
+        <v>-2</v>
+      </c>
+      <c r="AW31" s="3">
+        <v>32</v>
+      </c>
+      <c r="AX31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY31" s="3">
+        <v>1</v>
+      </c>
+      <c r="AZ31" s="3">
+        <v>0</v>
+      </c>
+      <c r="BA31" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB31" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC31" s="3">
+        <v>1</v>
+      </c>
+      <c r="BD31" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE31" s="3">
+        <v>7</v>
+      </c>
+      <c r="BF31" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG31" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="BH31" s="3">
+        <v>0</v>
+      </c>
+      <c r="BI31" s="3">
+        <v>500</v>
+      </c>
+      <c r="BJ31" s="3">
+        <v>3</v>
+      </c>
+      <c r="BK31" s="3">
+        <v>3</v>
+      </c>
+      <c r="BL31" s="3">
+        <v>3</v>
+      </c>
+      <c r="BM31" s="3">
+        <v>3</v>
+      </c>
+      <c r="BN31" s="3">
+        <v>3</v>
+      </c>
+      <c r="BO31" s="3">
+        <v>10</v>
+      </c>
+      <c r="BP31" s="3">
+        <v>4</v>
+      </c>
+      <c r="BQ31" s="3">
+        <v>4</v>
+      </c>
+      <c r="BR31" s="3">
+        <v>4</v>
+      </c>
+      <c r="BS31" s="3">
+        <v>4</v>
+      </c>
+      <c r="BT31" s="3">
+        <v>4</v>
+      </c>
+      <c r="BU31" s="3">
+        <v>4</v>
+      </c>
+      <c r="BV31" s="3">
+        <v>4</v>
+      </c>
+      <c r="BW31" s="3">
+        <v>10</v>
+      </c>
+      <c r="BX31" s="3">
+        <v>4</v>
+      </c>
+      <c r="BY31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="BZ31" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CA31" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="CB31" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="CC31" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="CD31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CE31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CF31" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CG31" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CH31" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CI31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CJ31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CK31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CL31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CM31" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CN31" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="CO31" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="CP31" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CQ31" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CR31" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CS31" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="CT31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CU31" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="CV31" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="CW31" s="3">
+        <v>3</v>
+      </c>
+      <c r="CX31" s="3">
+        <v>3</v>
+      </c>
+      <c r="CY31" s="3">
+        <v>3</v>
+      </c>
+      <c r="CZ31" s="3">
+        <v>3</v>
+      </c>
+      <c r="DA31" s="3">
+        <v>3</v>
+      </c>
+      <c r="DB31" s="3">
+        <v>10</v>
+      </c>
+      <c r="DC31" s="3">
+        <v>4</v>
+      </c>
+      <c r="DD31" s="3">
+        <v>4</v>
+      </c>
+      <c r="DE31" s="3">
+        <v>4</v>
+      </c>
+      <c r="DF31" s="3">
+        <v>4</v>
+      </c>
+      <c r="DG31" s="3">
+        <v>4</v>
+      </c>
+      <c r="DH31" s="3">
+        <v>4</v>
+      </c>
+      <c r="DI31" s="3">
+        <v>4</v>
+      </c>
+      <c r="DJ31" s="3">
+        <v>10</v>
+      </c>
+      <c r="DK31" s="3">
+        <v>4</v>
+      </c>
+      <c r="DL31" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32" t="s">
+        <v>187</v>
+      </c>
+      <c r="C32" s="4">
+        <v>54.45534</v>
+      </c>
+      <c r="D32" s="4">
+        <v>6.0879200000000004</v>
+      </c>
+      <c r="E32" s="12">
+        <v>40</v>
+      </c>
+      <c r="F32" s="1">
+        <v>45482</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2958465</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="J32" s="3">
+        <v>-20</v>
+      </c>
+      <c r="K32" s="3">
+        <v>20</v>
+      </c>
+      <c r="L32" s="3">
+        <v>-15</v>
+      </c>
+      <c r="M32" s="3">
+        <v>15</v>
+      </c>
+      <c r="N32" s="3">
+        <v>0</v>
+      </c>
+      <c r="O32" s="3">
+        <v>25</v>
+      </c>
+      <c r="P32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>40</v>
+      </c>
+      <c r="R32" s="3">
+        <v>0</v>
+      </c>
+      <c r="S32" s="3">
+        <v>40</v>
+      </c>
+      <c r="T32" s="3">
+        <v>0</v>
+      </c>
+      <c r="U32" s="3">
+        <v>25</v>
+      </c>
+      <c r="V32" s="3">
+        <v>0</v>
+      </c>
+      <c r="W32" s="3">
+        <v>25</v>
+      </c>
+      <c r="X32" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="3">
+        <v>30</v>
+      </c>
+      <c r="Z32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="3">
+        <v>25</v>
+      </c>
+      <c r="AB32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="3">
+        <v>30</v>
+      </c>
+      <c r="AD32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE32" s="3">
+        <v>30</v>
+      </c>
+      <c r="AF32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG32" s="3">
+        <v>25</v>
+      </c>
+      <c r="AH32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI32" s="3">
+        <v>30</v>
+      </c>
+      <c r="AJ32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK32" s="3">
+        <v>30</v>
+      </c>
+      <c r="AL32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM32" s="3">
+        <v>30</v>
+      </c>
+      <c r="AN32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AO32" s="3">
+        <v>30</v>
+      </c>
+      <c r="AP32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AQ32" s="3">
+        <v>30</v>
+      </c>
+      <c r="AR32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS32" s="3">
+        <v>360</v>
+      </c>
+      <c r="AT32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU32" s="3">
+        <v>360</v>
+      </c>
+      <c r="AV32" s="3">
+        <v>-2</v>
+      </c>
+      <c r="AW32" s="3">
+        <v>32</v>
+      </c>
+      <c r="AX32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AZ32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BA32" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BC32" s="3">
+        <v>1</v>
+      </c>
+      <c r="BD32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE32" s="3">
+        <v>7</v>
+      </c>
+      <c r="BF32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BG32" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="BH32" s="3">
+        <v>0</v>
+      </c>
+      <c r="BI32" s="3">
+        <v>500</v>
+      </c>
+      <c r="BJ32" s="3">
+        <v>3</v>
+      </c>
+      <c r="BK32" s="3">
+        <v>3</v>
+      </c>
+      <c r="BL32" s="3">
+        <v>3</v>
+      </c>
+      <c r="BM32" s="3">
+        <v>3</v>
+      </c>
+      <c r="BN32" s="3">
+        <v>3</v>
+      </c>
+      <c r="BO32" s="3">
+        <v>10</v>
+      </c>
+      <c r="BP32" s="3">
+        <v>4</v>
+      </c>
+      <c r="BQ32" s="3">
+        <v>4</v>
+      </c>
+      <c r="BR32" s="3">
+        <v>4</v>
+      </c>
+      <c r="BS32" s="3">
+        <v>4</v>
+      </c>
+      <c r="BT32" s="3">
+        <v>4</v>
+      </c>
+      <c r="BU32" s="3">
+        <v>4</v>
+      </c>
+      <c r="BV32" s="3">
+        <v>4</v>
+      </c>
+      <c r="BW32" s="3">
+        <v>10</v>
+      </c>
+      <c r="BX32" s="3">
+        <v>4</v>
+      </c>
+      <c r="BY32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="BZ32" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CA32" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="CB32" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="CC32" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="CD32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CE32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CF32" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CG32" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CH32" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CI32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CJ32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CK32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CL32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CM32" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CN32" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="CO32" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="CP32" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CQ32" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CR32" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="CS32" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="CT32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="CU32" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="CV32" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="CW32" s="3">
+        <v>3</v>
+      </c>
+      <c r="CX32" s="3">
+        <v>3</v>
+      </c>
+      <c r="CY32" s="3">
+        <v>3</v>
+      </c>
+      <c r="CZ32" s="3">
+        <v>3</v>
+      </c>
+      <c r="DA32" s="3">
+        <v>3</v>
+      </c>
+      <c r="DB32" s="3">
+        <v>10</v>
+      </c>
+      <c r="DC32" s="3">
+        <v>4</v>
+      </c>
+      <c r="DD32" s="3">
+        <v>4</v>
+      </c>
+      <c r="DE32" s="3">
+        <v>4</v>
+      </c>
+      <c r="DF32" s="3">
+        <v>4</v>
+      </c>
+      <c r="DG32" s="3">
+        <v>4</v>
+      </c>
+      <c r="DH32" s="3">
+        <v>4</v>
+      </c>
+      <c r="DI32" s="3">
+        <v>4</v>
+      </c>
+      <c r="DJ32" s="3">
+        <v>10</v>
+      </c>
+      <c r="DK32" s="3">
+        <v>4</v>
+      </c>
+      <c r="DL32" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="2"/>
+    </row>
   </sheetData>
-  <sortState ref="CZ7:DA21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="CZ7:DA21">
     <sortCondition ref="DA7:DA21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -11346,17 +12418,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CH24"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AS5" sqref="AS5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="41" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="13.125" hidden="1" customWidth="1"/>
+    <col min="3" max="41" width="11.625" hidden="1" customWidth="1"/>
     <col min="42" max="42" width="12.5" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="13" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="13.5" bestFit="1" customWidth="1"/>
@@ -11739,17 +12811,17 @@
       <c r="AO2" s="3">
         <v>500</v>
       </c>
-      <c r="AP2" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="AQ2" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="AR2" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="AS2" s="3">
-        <v>3.5</v>
+      <c r="AP2" s="7">
+        <v>-2</v>
+      </c>
+      <c r="AQ2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AR2" s="7">
+        <v>-2</v>
+      </c>
+      <c r="AS2" s="7">
+        <v>2</v>
       </c>
       <c r="AT2" s="3">
         <v>3</v>
@@ -11991,17 +13063,17 @@
       <c r="AO3" s="3">
         <v>500</v>
       </c>
-      <c r="AP3" s="3">
+      <c r="AP3" s="7">
         <v>-2</v>
       </c>
-      <c r="AQ3" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="AR3" s="3">
+      <c r="AQ3" s="7">
+        <v>2</v>
+      </c>
+      <c r="AR3" s="7">
         <v>-2</v>
       </c>
-      <c r="AS3" s="3">
-        <v>3.5</v>
+      <c r="AS3" s="7">
+        <v>2</v>
       </c>
       <c r="AT3" s="3">
         <v>3</v>
@@ -12247,13 +13319,13 @@
         <v>-1.5</v>
       </c>
       <c r="AQ4" s="20">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AR4" s="20">
         <v>-1.5</v>
       </c>
       <c r="AS4" s="20">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AT4" s="20">
         <v>3</v>
@@ -12496,16 +13568,16 @@
         <v>500</v>
       </c>
       <c r="AP5" s="7">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AQ5" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AR5" s="7">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AS5" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AT5" s="3">
         <v>3</v>
@@ -12748,16 +13820,16 @@
         <v>500</v>
       </c>
       <c r="AP6" s="7">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AQ6" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AR6" s="7">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AS6" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AT6" s="3">
         <v>3</v>
@@ -13000,16 +14072,16 @@
         <v>500</v>
       </c>
       <c r="AP7" s="7">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="AQ7" s="7">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AR7" s="7">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="AS7" s="7">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="AT7" s="3">
         <v>3</v>
@@ -13932,7 +15004,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BY5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15064,7 +16136,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:DU24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22982,7 +24054,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>